<commit_message>
edited more general version
</commit_message>
<xml_diff>
--- a/doc/conditions.xlsx
+++ b/doc/conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/japmiett/projects/neurocenter/clinicaltrials/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/japmiett/projects/neurocenter/clinicaltrialsAPI/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA39542E-341A-A248-9B4B-684F4E507E79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D5F11B-1799-1148-9493-F4019A9E8A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{2950F63C-1F2A-2549-BC3A-14330A7261B4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2950F63C-1F2A-2549-BC3A-14330A7261B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -549,15 +549,9 @@
     <t>Nervous System Diseases  </t>
   </si>
   <si>
-    <t>Condition</t>
-  </si>
-  <si>
     <t>Class</t>
   </si>
   <si>
-    <t>Cases</t>
-  </si>
-  <si>
     <t>Alcohol-Induced Disorders</t>
   </si>
   <si>
@@ -991,13 +985,19 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>Studies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1015,6 +1015,13 @@
     </font>
     <font>
       <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
@@ -1041,13 +1048,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1366,7 +1374,7 @@
   <dimension ref="A1:D340"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1378,16 +1386,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" t="s">
         <v>171</v>
       </c>
-      <c r="C1" t="s">
-        <v>173</v>
+      <c r="B1" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>318</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1401,7 +1409,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1415,7 +1423,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1429,7 +1437,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1443,7 +1451,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1457,7 +1465,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1471,7 +1479,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1485,7 +1493,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1499,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1513,7 +1521,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1527,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1541,7 +1549,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1555,7 +1563,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1569,7 +1577,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1583,7 +1591,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1597,7 +1605,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1611,7 +1619,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1625,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1639,7 +1647,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1653,7 +1661,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1667,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1681,7 +1689,7 @@
         <v>12</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1695,7 +1703,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1709,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1723,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1737,7 +1745,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1751,7 +1759,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1765,7 +1773,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1779,7 +1787,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1793,7 +1801,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1807,7 +1815,7 @@
         <v>7</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1821,7 +1829,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1835,7 +1843,7 @@
         <v>1</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1849,7 +1857,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1863,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1877,7 +1885,7 @@
         <v>41</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1891,7 +1899,7 @@
         <v>10</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1905,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1919,7 +1927,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1933,7 +1941,7 @@
         <v>5</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1947,7 +1955,7 @@
         <v>12</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1961,7 +1969,7 @@
         <v>3</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1975,7 +1983,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1989,7 +1997,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -2003,7 +2011,7 @@
         <v>7</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -2017,7 +2025,7 @@
         <v>1</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -2031,7 +2039,7 @@
         <v>1</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -2045,7 +2053,7 @@
         <v>41</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -2059,7 +2067,7 @@
         <v>24</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -2073,7 +2081,7 @@
         <v>4</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -2087,7 +2095,7 @@
         <v>4</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -2101,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -2115,7 +2123,7 @@
         <v>7</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2129,7 +2137,7 @@
         <v>2</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -2143,7 +2151,7 @@
         <v>7</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2157,7 +2165,7 @@
         <v>1</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -2171,7 +2179,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -2185,7 +2193,7 @@
         <v>4</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2199,7 +2207,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -2213,7 +2221,7 @@
         <v>10</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2227,7 +2235,7 @@
         <v>2</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2241,7 +2249,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2255,7 +2263,7 @@
         <v>18</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2269,7 +2277,7 @@
         <v>1</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2283,7 +2291,7 @@
         <v>2</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2297,7 +2305,7 @@
         <v>1</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2311,7 +2319,7 @@
         <v>2</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2325,7 +2333,7 @@
         <v>1</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2339,7 +2347,7 @@
         <v>60</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2353,7 +2361,7 @@
         <v>2</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2367,7 +2375,7 @@
         <v>2</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2381,7 +2389,7 @@
         <v>1</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2395,7 +2403,7 @@
         <v>9</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2409,7 +2417,7 @@
         <v>8</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2423,7 +2431,7 @@
         <v>5</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2437,7 +2445,7 @@
         <v>10</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2451,7 +2459,7 @@
         <v>4</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2465,7 +2473,7 @@
         <v>2</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2479,7 +2487,7 @@
         <v>68</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2493,7 +2501,7 @@
         <v>3</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2507,7 +2515,7 @@
         <v>2</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2521,7 +2529,7 @@
         <v>8</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -2535,7 +2543,7 @@
         <v>1</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -2549,7 +2557,7 @@
         <v>2</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -2563,7 +2571,7 @@
         <v>27</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -2577,7 +2585,7 @@
         <v>1</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -2591,7 +2599,7 @@
         <v>2</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2605,7 +2613,7 @@
         <v>1</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -2619,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -2633,7 +2641,7 @@
         <v>1</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2647,7 +2655,7 @@
         <v>9</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -2661,7 +2669,7 @@
         <v>1</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2675,7 +2683,7 @@
         <v>1</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2689,7 +2697,7 @@
         <v>10</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -2703,7 +2711,7 @@
         <v>18</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -2717,7 +2725,7 @@
         <v>18</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -2731,7 +2739,7 @@
         <v>2</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -2745,7 +2753,7 @@
         <v>1</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -2759,7 +2767,7 @@
         <v>1</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -2773,7 +2781,7 @@
         <v>7</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -2787,7 +2795,7 @@
         <v>1</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -2801,7 +2809,7 @@
         <v>3</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -2815,7 +2823,7 @@
         <v>1</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -2829,7 +2837,7 @@
         <v>2</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -2843,7 +2851,7 @@
         <v>1</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -2857,7 +2865,7 @@
         <v>1</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -2871,7 +2879,7 @@
         <v>1</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -2885,7 +2893,7 @@
         <v>3</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -2899,7 +2907,7 @@
         <v>2</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -2913,7 +2921,7 @@
         <v>2</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -2927,7 +2935,7 @@
         <v>8</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -2941,7 +2949,7 @@
         <v>8</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2955,7 +2963,7 @@
         <v>1</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -2969,7 +2977,7 @@
         <v>1</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -2983,7 +2991,7 @@
         <v>1</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -2997,7 +3005,7 @@
         <v>1</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -3011,7 +3019,7 @@
         <v>1</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -3025,7 +3033,7 @@
         <v>3</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -3039,7 +3047,7 @@
         <v>2</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -3053,7 +3061,7 @@
         <v>1</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -3067,7 +3075,7 @@
         <v>5</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -3081,7 +3089,7 @@
         <v>5</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -3095,7 +3103,7 @@
         <v>1</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -3109,7 +3117,7 @@
         <v>7</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -3123,7 +3131,7 @@
         <v>3</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -3137,7 +3145,7 @@
         <v>1</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -3151,7 +3159,7 @@
         <v>2</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -3165,7 +3173,7 @@
         <v>1</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -3179,7 +3187,7 @@
         <v>1</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -3193,7 +3201,7 @@
         <v>1</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -3207,7 +3215,7 @@
         <v>2</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -3221,7 +3229,7 @@
         <v>1</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -3235,7 +3243,7 @@
         <v>8</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -3249,7 +3257,7 @@
         <v>1</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -3263,7 +3271,7 @@
         <v>1</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -3277,7 +3285,7 @@
         <v>2</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -3291,7 +3299,7 @@
         <v>18</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -3305,7 +3313,7 @@
         <v>2</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -3319,7 +3327,7 @@
         <v>2</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -3333,7 +3341,7 @@
         <v>1</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -3347,7 +3355,7 @@
         <v>1</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -3361,7 +3369,7 @@
         <v>9</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -3375,7 +3383,7 @@
         <v>1</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -3389,7 +3397,7 @@
         <v>2</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -3403,7 +3411,7 @@
         <v>3</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -3417,7 +3425,7 @@
         <v>3</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -3431,7 +3439,7 @@
         <v>5</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -3445,7 +3453,7 @@
         <v>1</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -3459,7 +3467,7 @@
         <v>11</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -3473,7 +3481,7 @@
         <v>41</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -3487,7 +3495,7 @@
         <v>9</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -3501,7 +3509,7 @@
         <v>1</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -3515,7 +3523,7 @@
         <v>1</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -3529,7 +3537,7 @@
         <v>1</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -3543,7 +3551,7 @@
         <v>3</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -3557,7 +3565,7 @@
         <v>7</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -3571,7 +3579,7 @@
         <v>2</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -3585,7 +3593,7 @@
         <v>2</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -3599,7 +3607,7 @@
         <v>5</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -3613,7 +3621,7 @@
         <v>1</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -3627,7 +3635,7 @@
         <v>1</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -3641,7 +3649,7 @@
         <v>1</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -3655,7 +3663,7 @@
         <v>1</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -3669,7 +3677,7 @@
         <v>1</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -3683,7 +3691,7 @@
         <v>1</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -3697,7 +3705,7 @@
         <v>1</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -3711,7 +3719,7 @@
         <v>1</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -3725,7 +3733,7 @@
         <v>3</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -3739,7 +3747,7 @@
         <v>1</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -3753,7 +3761,7 @@
         <v>3</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -3767,7 +3775,7 @@
         <v>3</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -3781,7 +3789,7 @@
         <v>1</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
@@ -3795,7 +3803,7 @@
         <v>7</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -3809,7 +3817,7 @@
         <v>2</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
@@ -3823,7 +3831,7 @@
         <v>7</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -3837,7 +3845,7 @@
         <v>1</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
@@ -3851,7 +3859,7 @@
         <v>1</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -3865,7 +3873,7 @@
         <v>2</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -3879,7 +3887,7 @@
         <v>3</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
@@ -3893,7 +3901,7 @@
         <v>2</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -3907,7 +3915,7 @@
         <v>1</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
@@ -3921,7 +3929,7 @@
         <v>25</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
@@ -3935,7 +3943,7 @@
         <v>4</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -3949,7 +3957,7 @@
         <v>8</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
@@ -3963,7 +3971,7 @@
         <v>1</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
@@ -3977,7 +3985,7 @@
         <v>1</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
@@ -3991,7 +3999,7 @@
         <v>11</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
@@ -4005,7 +4013,7 @@
         <v>2</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -4019,26 +4027,26 @@
         <v>2</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C190">
         <v>1</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>2</v>
@@ -4047,12 +4055,12 @@
         <v>3</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>3</v>
@@ -4061,68 +4069,68 @@
         <v>2</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C193">
         <v>1</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C194">
         <v>6</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C195">
         <v>1</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C196">
         <v>1</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>33</v>
@@ -4131,12 +4139,12 @@
         <v>1</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>137</v>
@@ -4145,40 +4153,40 @@
         <v>1</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C199">
         <v>1</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C200">
         <v>1</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>56</v>
@@ -4187,138 +4195,138 @@
         <v>4</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C202" s="2">
         <v>2</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C203" s="2">
         <v>22</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C204" s="2">
         <v>1</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C205" s="2">
         <v>1</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C206" s="2">
         <v>1</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C207" s="2">
         <v>3</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C208" s="2">
         <v>1</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C209" s="2">
         <v>1</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C210" s="2">
         <v>1</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>73</v>
@@ -4327,222 +4335,222 @@
         <v>4</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C212" s="2">
         <v>24</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C213" s="2">
         <v>11</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C214" s="2">
         <v>1</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C215" s="2">
         <v>56</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C216" s="2">
         <v>3</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="217" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C217" s="2">
         <v>1</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="218" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C218" s="2">
         <v>11</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="219" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C219" s="2">
         <v>2</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C220" s="2">
         <v>2</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C221" s="2">
         <v>2</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C222" s="2">
         <v>15</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C223" s="2">
         <v>17</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C224" s="2">
         <v>11</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C225" s="2">
         <v>2</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C226" s="2">
         <v>5</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>75</v>
@@ -4551,376 +4559,376 @@
         <v>3</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C228" s="2">
         <v>3</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C229" s="2">
         <v>3</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="230" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C230" s="2">
         <v>5</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C231" s="2">
         <v>15</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="232" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C232" s="2">
         <v>1</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C233" s="2">
         <v>2</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="234" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C234" s="2">
         <v>26</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="235" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C235" s="2">
         <v>1</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C236" s="2">
         <v>21</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C237" s="2">
         <v>3</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C238" s="2">
         <v>1</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C239" s="2">
         <v>6</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="240" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C240" s="2">
         <v>1</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C241" s="2">
         <v>1</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="242" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C242" s="2">
         <v>2</v>
       </c>
       <c r="D242" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="243" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C243" s="2">
         <v>1</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C244" s="2">
         <v>26</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="245" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C245" s="2">
         <v>2</v>
       </c>
       <c r="D245" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C246" s="2">
         <v>19</v>
       </c>
       <c r="D246" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C247" s="2">
         <v>38</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C248" s="2">
         <v>3</v>
       </c>
       <c r="D248" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="249" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C249" s="2">
         <v>4</v>
       </c>
       <c r="D249" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="250" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C250" s="2">
         <v>7</v>
       </c>
       <c r="D250" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="251" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C251" s="2">
         <v>1</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C252" s="2">
         <v>2</v>
       </c>
       <c r="D252" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C253" s="2">
         <v>1</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>108</v>
@@ -4929,684 +4937,684 @@
         <v>1</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C255" s="2">
         <v>15</v>
       </c>
       <c r="D255" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="256" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C256" s="2">
         <v>11</v>
       </c>
       <c r="D256" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C257" s="2">
         <v>4</v>
       </c>
       <c r="D257" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C258" s="2">
         <v>1</v>
       </c>
       <c r="D258" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C259" s="2">
         <v>35</v>
       </c>
       <c r="D259" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C260" s="2">
         <v>5</v>
       </c>
       <c r="D260" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C261" s="2">
         <v>5</v>
       </c>
       <c r="D261" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="262" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C262" s="2">
         <v>17</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C263" s="2">
         <v>4</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C264" s="2">
         <v>17</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C265" s="2">
         <v>12</v>
       </c>
       <c r="D265" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C266" s="2">
         <v>1</v>
       </c>
       <c r="D266" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C267" s="2">
         <v>1</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C268" s="2">
         <v>1</v>
       </c>
       <c r="D268" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C269" s="2">
         <v>1</v>
       </c>
       <c r="D269" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="270" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C270" s="2">
         <v>1</v>
       </c>
       <c r="D270" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C271" s="2">
         <v>1</v>
       </c>
       <c r="D271" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="272" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C272" s="2">
         <v>2</v>
       </c>
       <c r="D272" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="273" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C273" s="2">
         <v>16</v>
       </c>
       <c r="D273" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C274" s="2">
         <v>29</v>
       </c>
       <c r="D274" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C275" s="2">
         <v>9</v>
       </c>
       <c r="D275" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C276" s="2">
         <v>1</v>
       </c>
       <c r="D276" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C277" s="2">
         <v>5</v>
       </c>
       <c r="D277" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C278" s="2">
         <v>6</v>
       </c>
       <c r="D278" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C279" s="2">
         <v>2</v>
       </c>
       <c r="D279" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="280" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C280" s="2">
         <v>17</v>
       </c>
       <c r="D280" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C281" s="2">
         <v>11</v>
       </c>
       <c r="D281" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="282" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C282" s="2">
         <v>2</v>
       </c>
       <c r="D282" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="283" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C283" s="2">
         <v>7</v>
       </c>
       <c r="D283" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="284" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C284" s="2">
         <v>4</v>
       </c>
       <c r="D284" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="285" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C285" s="2">
         <v>19</v>
       </c>
       <c r="D285" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="286" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C286" s="2">
         <v>4</v>
       </c>
       <c r="D286" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C287" s="2">
         <v>119</v>
       </c>
       <c r="D287" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="288" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C288" s="2">
         <v>1</v>
       </c>
       <c r="D288" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="289" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C289" s="2">
         <v>1</v>
       </c>
       <c r="D289" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="290" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C290" s="2">
         <v>10</v>
       </c>
       <c r="D290" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C291" s="2">
         <v>6</v>
       </c>
       <c r="D291" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="292" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C292" s="2">
         <v>1</v>
       </c>
       <c r="D292" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C293" s="2">
         <v>18</v>
       </c>
       <c r="D293" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C294" s="2">
         <v>45</v>
       </c>
       <c r="D294" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="295" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A295" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C295" s="2">
         <v>1</v>
       </c>
       <c r="D295" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C296" s="2">
         <v>18</v>
       </c>
       <c r="D296" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A297" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C297" s="2">
         <v>4</v>
       </c>
       <c r="D297" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="298" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C298" s="2">
         <v>7</v>
       </c>
       <c r="D298" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C299" s="2">
         <v>2</v>
       </c>
       <c r="D299" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="300" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C300" s="2">
         <v>2</v>
       </c>
       <c r="D300" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C301" s="2">
         <v>1</v>
       </c>
       <c r="D301" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C302" s="2">
         <v>10</v>
       </c>
       <c r="D302" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A303" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B303" s="1" t="s">
         <v>130</v>
@@ -5615,12 +5623,12 @@
         <v>3</v>
       </c>
       <c r="D303" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B304" s="1" t="s">
         <v>132</v>
@@ -5629,511 +5637,511 @@
         <v>1</v>
       </c>
       <c r="D304" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C305" s="2">
         <v>17</v>
       </c>
       <c r="D305" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="306" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C306" s="2">
         <v>17</v>
       </c>
       <c r="D306" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A307" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C307" s="2">
         <v>13</v>
       </c>
       <c r="D307" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="308" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C308" s="2">
         <v>10</v>
       </c>
       <c r="D308" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C309" s="2">
         <v>10</v>
       </c>
       <c r="D309" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C310" s="2">
         <v>10</v>
       </c>
       <c r="D310" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C311" s="2">
         <v>1</v>
       </c>
       <c r="D311" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="312" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C312" s="2">
         <v>2</v>
       </c>
       <c r="D312" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="313" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A313" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C313" s="2">
         <v>1</v>
       </c>
       <c r="D313" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="314" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A314" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C314" s="2">
         <v>17</v>
       </c>
       <c r="D314" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="315" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A315" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C315" s="2">
         <v>8</v>
       </c>
       <c r="D315" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A316" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C316" s="2">
         <v>1</v>
       </c>
       <c r="D316" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A317" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C317" s="2">
         <v>2</v>
       </c>
       <c r="D317" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="318" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A318" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C318" s="2">
         <v>6</v>
       </c>
       <c r="D318" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="319" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A319" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C319" s="2">
         <v>11</v>
       </c>
       <c r="D319" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="320" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A320" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C320" s="2">
         <v>2</v>
       </c>
       <c r="D320" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="321" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A321" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C321" s="2">
         <v>7</v>
       </c>
       <c r="D321" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="322" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C322" s="2">
         <v>39</v>
       </c>
       <c r="D322" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A323" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C323" s="2">
         <v>6</v>
       </c>
       <c r="D323" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="324" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C324" s="2">
         <v>13</v>
       </c>
       <c r="D324" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="325" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C325" s="2">
         <v>3</v>
       </c>
       <c r="D325" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="326" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C326" s="2">
         <v>2</v>
       </c>
       <c r="D326" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="327" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A327" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C327" s="2">
         <v>2</v>
       </c>
       <c r="D327" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="328" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A328" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C328" s="2">
         <v>1</v>
       </c>
       <c r="D328" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="329" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A329" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C329" s="2">
         <v>2</v>
       </c>
       <c r="D329" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="330" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A330" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C330" s="2">
         <v>2</v>
       </c>
       <c r="D330" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="331" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A331" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C331" s="2">
         <v>1</v>
       </c>
       <c r="D331" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A332" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C332" s="2">
         <v>14</v>
       </c>
       <c r="D332" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="333" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A333" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C333" s="2">
         <v>1</v>
       </c>
       <c r="D333" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="334" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A334" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C334" s="2">
         <v>4</v>
       </c>
       <c r="D334" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="335" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A335" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C335" s="2">
         <v>11</v>
       </c>
       <c r="D335" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="336" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A336" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C336" s="2">
         <v>75</v>
       </c>
       <c r="D336" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="337" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A337" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C337" s="2">
         <v>19</v>
       </c>
       <c r="D337" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="338" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A338" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C338" s="2">
         <v>1</v>
       </c>
       <c r="D338" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="339" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A339" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C339" s="2">
         <v>1</v>
       </c>
       <c r="D339" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="340" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C340" s="2">
         <v>4</v>
       </c>
       <c r="D340" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>